<commit_message>
Addresses import by sheet name #26
</commit_message>
<xml_diff>
--- a/src/NetCore.Utilities.Spreadsheet.Tests/SampleFiles/ImportSample.xlsx
+++ b/src/NetCore.Utilities.Spreadsheet.Tests/SampleFiles/ImportSample.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\ICG-Git\Repos\netcore.utilities.spreadsheet\src\NetCore.Utilities.Spreadsheet.Tests\SampleFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\netcore.utilities.spreadsheet\src\NetCore.Utilities.Spreadsheet.Tests\SampleFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5751F63B-39D1-4635-8928-700B27907BBD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD2D022-9B35-4A3D-8B02-364A48398C37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1837" yWindow="1837" windowWidth="21600" windowHeight="11423" xr2:uid="{276BD12E-2F60-451D-BE70-71D9839A872B}"/>
+    <workbookView xWindow="28995" yWindow="2145" windowWidth="22005" windowHeight="16200" activeTab="1" xr2:uid="{276BD12E-2F60-451D-BE70-71D9839A872B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Test Sheet" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
   <si>
     <t>Name</t>
   </si>
@@ -46,6 +47,9 @@
   </si>
   <si>
     <t>Jill Smith</t>
+  </si>
+  <si>
+    <t>Adam</t>
   </si>
 </sst>
 </file>
@@ -399,13 +403,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97DD670-D257-4816-A774-A2EEBC5FD74D}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -413,7 +417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -421,12 +425,59 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
         <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D830C04C-B3F3-4446-87F5-F824A0C59549}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>